<commit_message>
Increased xp needed for leveling
</commit_message>
<xml_diff>
--- a/AdjustableLeveling.xlsx
+++ b/AdjustableLeveling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0Stuff\MB2_Bannerlord\AdjustableLeveling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205244BB-9485-4960-908F-F93E9E0EE309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F0308B-FEDA-412C-90F3-3070643FD588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{7387DAE2-B7E8-4465-A8E3-EFF996C1B00C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{7387DAE2-B7E8-4465-A8E3-EFF996C1B00C}"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Original</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Adjustable</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -165,12 +168,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="2"/>
@@ -19954,187 +19952,187 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3009.8491553067593</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4537.54050759853</c:v>
+                  <c:v>675</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6097.0058602566651</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7702.5820745865949</c:v>
+                  <c:v>3125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9369.742289632497</c:v>
+                  <c:v>5400</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11114.926957144702</c:v>
+                  <c:v>8575</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12955.425783333691</c:v>
+                  <c:v>12800</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14909.289710755254</c:v>
+                  <c:v>18225</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16995.262314968881</c:v>
+                  <c:v>25000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19232.724566579924</c:v>
+                  <c:v>33275</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21641.649234067241</c:v>
+                  <c:v>43200</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24242.562496194205</c:v>
+                  <c:v>54925</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27056.511103231107</c:v>
+                  <c:v>68600</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>30105.033910343955</c:v>
+                  <c:v>84375</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33410.136924135702</c:v>
+                  <c:v>102400</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36994.271219276969</c:v>
+                  <c:v>122825</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40880.313233446432</c:v>
+                  <c:v>145800</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>45091.547057523356</c:v>
+                  <c:v>171475</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>49651.648417852644</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>54584.670107231352</c:v>
+                  <c:v>231525</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>59915.02866684222</c:v>
+                  <c:v>266200</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>65667.492156608074</c:v>
+                  <c:v>304175</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>71867.168879069475</c:v>
+                  <c:v>345600</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>78539.496943808801</c:v>
+                  <c:v>390625</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>85710.234577028983</c:v>
+                  <c:v>439400</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>93405.451095137178</c:v>
+                  <c:v>492075</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>101651.51847283544</c:v>
+                  <c:v>548800</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>110475.10344581748</c:v>
+                  <c:v>609725</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>119903.16009614893</c:v>
+                  <c:v>675000</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>129962.92287508317</c:v>
+                  <c:v>744775</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>140681.90002368303</c:v>
+                  <c:v>819200</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>152087.86735638179</c:v>
+                  <c:v>898425</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>164208.86237667289</c:v>
+                  <c:v>982600</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>177073.17869759607</c:v>
+                  <c:v>1071875</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>190709.36074268064</c:v>
+                  <c:v>1166400</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>205146.19870558815</c:v>
+                  <c:v>1266325</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>220412.7237489532</c:v>
+                  <c:v>1371800</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>236538.20342487987</c:v>
+                  <c:v>1482975</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>253552.13730126186</c:v>
+                  <c:v>1600000</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>271484.25277961418</c:v>
+                  <c:v>1723025</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>290364.50109142601</c:v>
+                  <c:v>1852200</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>310223.05346122826</c:v>
+                  <c:v>1987675</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>331090.29742560833</c:v>
+                  <c:v>2129600</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>352996.83329834224</c:v>
+                  <c:v>2278125</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>375973.47077263665</c:v>
+                  <c:v>2433400</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>400051.22565222369</c:v>
+                  <c:v>2595575</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>425261.31670371996</c:v>
+                  <c:v>2764800</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>451635.16262324178</c:v>
+                  <c:v>2941225</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>479204.37911084824</c:v>
+                  <c:v>3125000</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>508000.77604682645</c:v>
+                  <c:v>3316275</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>538056.35476431798</c:v>
+                  <c:v>3515200</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>569403.30541315547</c:v>
+                  <c:v>3721925</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>602074.00441016629</c:v>
+                  <c:v>3936600</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>636101.01197151467</c:v>
+                  <c:v>4159375</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>671517.06972298003</c:v>
+                  <c:v>4390400</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>708355.0983843162</c:v>
+                  <c:v>4629825</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>746648.19552412792</c:v>
+                  <c:v>4877800</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>786429.63338189654</c:v>
+                  <c:v>5134475</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>827732.85675402719</c:v>
+                  <c:v>5400000</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>870591.48094099003</c:v>
+                  <c:v>5674525</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>915039.28975276963</c:v>
+                  <c:v>5958200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20143,6 +20141,228 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000E-45D8-4631-BF64-4DE34945AA1B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Level!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Level!$I$2:$I$64</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="63"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>72000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>84500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>98000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>144500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>162000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>180500</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>220500</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>242000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>264500</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>288000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>312500</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>338000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>364500</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>392000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>420500</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>450000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>480500</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>512000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>544500</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>578000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>612500</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>648000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>684500</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>722000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>760500</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>840500</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>882000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>924500</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>968000</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1012500</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1058000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1104500</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1152000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1200500</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1250000</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1300500</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1352000</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1404500</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1458000</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1512500</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1568000</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1624500</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1682000</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1740500</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1800000</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1860500</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1922000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D31-4D8A-865C-9FDA2F639C72}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -20212,7 +20432,7 @@
         <c:axId val="88987743"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1000000"/>
+          <c:max val="6000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -20880,187 +21100,187 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3010.8491553067593</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7548.3896629052888</c:v>
+                  <c:v>876</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13645.395523161955</c:v>
+                  <c:v>2476</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21347.977597748548</c:v>
+                  <c:v>5601</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30717.719887381045</c:v>
+                  <c:v>11001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41832.646844525749</c:v>
+                  <c:v>19576</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>54788.072627859437</c:v>
+                  <c:v>32376</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>69697.362338614694</c:v>
+                  <c:v>50601</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>86692.624653583567</c:v>
+                  <c:v>75601</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>105925.34922016349</c:v>
+                  <c:v>108876</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>127566.99845423074</c:v>
+                  <c:v>152076</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>151809.56095042493</c:v>
+                  <c:v>207001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>178866.07205365604</c:v>
+                  <c:v>275601</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>208971.10596399999</c:v>
+                  <c:v>359976</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>242381.24288813569</c:v>
+                  <c:v>462376</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>279375.51410741266</c:v>
+                  <c:v>585201</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>320255.8273408591</c:v>
+                  <c:v>731001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>365347.37439838244</c:v>
+                  <c:v>902476</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>414999.02281623508</c:v>
+                  <c:v>1102476</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>469583.69292346644</c:v>
+                  <c:v>1334001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>529498.72159030871</c:v>
+                  <c:v>1600201</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>595166.21374691674</c:v>
+                  <c:v>1904376</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>667033.38262598624</c:v>
+                  <c:v>2249976</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>745572.87956979498</c:v>
+                  <c:v>2640601</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>831283.11414682399</c:v>
+                  <c:v>3080001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>924688.56524196116</c:v>
+                  <c:v>3572076</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1026340.0837147966</c:v>
+                  <c:v>4120876</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1136815.1871606139</c:v>
+                  <c:v>4730601</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1256718.3472567629</c:v>
+                  <c:v>5405601</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1386681.270131846</c:v>
+                  <c:v>6150376</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1527363.1701555289</c:v>
+                  <c:v>6969576</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1679451.0375119108</c:v>
+                  <c:v>7868001</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1843659.8998885837</c:v>
+                  <c:v>8850601</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2020733.0785861798</c:v>
+                  <c:v>9922476</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2211442.4393288605</c:v>
+                  <c:v>11088876</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2416588.6380344485</c:v>
+                  <c:v>12355201</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2637001.3617834016</c:v>
+                  <c:v>13727001</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2873539.5652082814</c:v>
+                  <c:v>15209976</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3127091.7025095434</c:v>
+                  <c:v>16809976</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3398575.9552891576</c:v>
+                  <c:v>18533001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3688940.4563805833</c:v>
+                  <c:v>20385201</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3999163.5098418118</c:v>
+                  <c:v>22372876</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4330253.80726742</c:v>
+                  <c:v>24502476</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4683250.6405657623</c:v>
+                  <c:v>26780601</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5059224.1113383994</c:v>
+                  <c:v>29214001</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>5459275.3369906228</c:v>
+                  <c:v>31809576</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>5884536.6536943428</c:v>
+                  <c:v>34574376</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>6336171.8163175844</c:v>
+                  <c:v>37515601</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6815376.1954284329</c:v>
+                  <c:v>40640601</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>7323376.9714752594</c:v>
+                  <c:v>43956876</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>7861433.3262395775</c:v>
+                  <c:v>47472076</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>8430836.6316527333</c:v>
+                  <c:v>51194001</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>9032910.6360628996</c:v>
+                  <c:v>55130601</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>9669011.6480344143</c:v>
+                  <c:v>59289976</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>10340528.717757395</c:v>
+                  <c:v>63680376</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>11048883.816141712</c:v>
+                  <c:v>68310201</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>11795532.01166584</c:v>
+                  <c:v>73188001</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>12581961.645047735</c:v>
+                  <c:v>78322476</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>13409694.501801763</c:v>
+                  <c:v>83722476</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>14280285.982742753</c:v>
+                  <c:v>89397001</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>15195325.272495523</c:v>
+                  <c:v>95355201</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21069,6 +21289,237 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-E73F-464D-B007-E513D7002088}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Level!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Level!$J$2:$J$64</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="63"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14501</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>69501</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>101501</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>142001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>192001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>252501</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>324501</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>409001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>507001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>619501</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>747501</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>892001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1054001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1234501</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1434501</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1655001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1897001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2161501</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2449501</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2762001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3100001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3464501</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3856501</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4277001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4727001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5207501</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5719501</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6264001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6842001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7454501</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8102501</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8787001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9509001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10269501</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>11069501</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>11910001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12792001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>13716501</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>14684501</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>15697001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>16755001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>17859501</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>19011501</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20212001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>21462001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>22762501</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>24114501</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>25519001</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>26977001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>28489501</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>30057501</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>31682001</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>33364001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>35104501</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>36904501</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>38765001</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>40687001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3B8F-46F3-AB19-F1A7848A8780}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -21138,7 +21589,7 @@
         <c:axId val="88987743"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="16000000"/>
+          <c:max val="100000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -47900,11 +48351,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5330C290-746D-4873-BDF2-B5713C60EB14}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S52" sqref="S52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47915,7 +48366,7 @@
     <col min="5" max="8" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
@@ -47929,8 +48380,12 @@
         <v>3</v>
       </c>
       <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="14"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -47953,8 +48408,14 @@
       <c r="H2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -47979,8 +48440,15 @@
         <f>G3+G2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <f>I3+I2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -48004,15 +48472,23 @@
         <v>2002</v>
       </c>
       <c r="G4" s="2">
-        <f>A4^$G$67+A4*$G$66</f>
-        <v>3009.8491553067593</v>
+        <f t="shared" ref="G4:G63" si="2">$G$66*A4^$G$67</f>
+        <v>200</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="1"/>
-        <v>3010.8491553067593</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" ref="I4:I63" si="3">$I$66*A4^$I$67</f>
+        <v>2000</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J64" si="4">I4+J3</f>
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -48021,7 +48497,7 @@
         <v>2200</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ref="C5:C6" si="2">C4+B5</f>
+        <f t="shared" ref="C5:C6" si="5">C4+B5</f>
         <v>3201</v>
       </c>
       <c r="D5" s="2">
@@ -48029,7 +48505,7 @@
         <v>4203</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E64" si="3">E4+2000</f>
+        <f t="shared" ref="E5:E65" si="6">E4+2000</f>
         <v>4001</v>
       </c>
       <c r="F5" s="2">
@@ -48037,24 +48513,32 @@
         <v>6003</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ref="G5:G64" si="4">A5^$G$67+A5*$G$66</f>
-        <v>4537.54050759853</v>
+        <f t="shared" si="2"/>
+        <v>675</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="1"/>
-        <v>7548.3896629052888</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>876</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="3"/>
+        <v>4500</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="4"/>
+        <v>6501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <f t="shared" ref="B6:B64" si="5">B5+1000+B5/5</f>
+        <f t="shared" ref="B6:B65" si="7">B5+1000+B5/5</f>
         <v>3640</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6841</v>
       </c>
       <c r="D6" s="2">
@@ -48062,7 +48546,7 @@
         <v>11044</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6001</v>
       </c>
       <c r="F6" s="2">
@@ -48070,24 +48554,32 @@
         <v>12004</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="4"/>
-        <v>6097.0058602566651</v>
+        <f t="shared" si="2"/>
+        <v>1600</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="1"/>
-        <v>13645.395523161955</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2476</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="3"/>
+        <v>8000</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="4"/>
+        <v>14501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5368</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" ref="C7:C64" si="6">C6+B7</f>
+        <f t="shared" ref="C7:C64" si="8">C6+B7</f>
         <v>12209</v>
       </c>
       <c r="D7" s="2">
@@ -48095,7 +48587,7 @@
         <v>23253</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>8001</v>
       </c>
       <c r="F7" s="2">
@@ -48103,24 +48595,32 @@
         <v>20005</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="4"/>
-        <v>7702.5820745865949</v>
+        <f t="shared" si="2"/>
+        <v>3125</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="1"/>
-        <v>21347.977597748548</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5601</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="3"/>
+        <v>12500</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="4"/>
+        <v>27001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7441.6</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19650.599999999999</v>
       </c>
       <c r="D8" s="2">
@@ -48128,7 +48628,7 @@
         <v>42903.6</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>10001</v>
       </c>
       <c r="F8" s="2">
@@ -48136,24 +48636,32 @@
         <v>30006</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="4"/>
-        <v>9369.742289632497</v>
+        <f t="shared" si="2"/>
+        <v>5400</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="1"/>
-        <v>30717.719887381045</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>11001</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="3"/>
+        <v>18000</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="4"/>
+        <v>45001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9929.92</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>29580.519999999997</v>
       </c>
       <c r="D9" s="2">
@@ -48161,7 +48669,7 @@
         <v>72484.12</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>12001</v>
       </c>
       <c r="F9" s="2">
@@ -48169,24 +48677,32 @@
         <v>42007</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="4"/>
-        <v>11114.926957144702</v>
+        <f t="shared" si="2"/>
+        <v>8575</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="1"/>
-        <v>41832.646844525749</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19576</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="3"/>
+        <v>24500</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="4"/>
+        <v>69501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>12915.904</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>42496.423999999999</v>
       </c>
       <c r="D10" s="2">
@@ -48194,7 +48710,7 @@
         <v>114980.54399999999</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>14001</v>
       </c>
       <c r="F10" s="2">
@@ -48202,24 +48718,32 @@
         <v>56008</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="4"/>
-        <v>12955.425783333691</v>
+        <f t="shared" si="2"/>
+        <v>12800</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="1"/>
-        <v>54788.072627859437</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32376</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="3"/>
+        <v>32000</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="4"/>
+        <v>101501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>16499.084800000001</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>58995.508799999996</v>
       </c>
       <c r="D11" s="2">
@@ -48227,7 +48751,7 @@
         <v>173976.0528</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>16001</v>
       </c>
       <c r="F11" s="2">
@@ -48235,24 +48759,32 @@
         <v>72009</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="4"/>
-        <v>14909.289710755254</v>
+        <f t="shared" si="2"/>
+        <v>18225</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="1"/>
-        <v>69697.362338614694</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>50601</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="3"/>
+        <v>40500</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="4"/>
+        <v>142001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>20798.901760000001</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>79794.410559999989</v>
       </c>
       <c r="D12" s="2">
@@ -48260,7 +48792,7 @@
         <v>253770.46335999999</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>18001</v>
       </c>
       <c r="F12" s="2">
@@ -48268,24 +48800,32 @@
         <v>90010</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="4"/>
-        <v>16995.262314968881</v>
+        <f t="shared" si="2"/>
+        <v>25000</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="1"/>
-        <v>86692.624653583567</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>75601</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="3"/>
+        <v>50000</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="4"/>
+        <v>192001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>25958.682112000002</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>105753.092672</v>
       </c>
       <c r="D13" s="2">
@@ -48293,7 +48833,7 @@
         <v>359523.55603199999</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>20001</v>
       </c>
       <c r="F13" s="2">
@@ -48301,24 +48841,32 @@
         <v>110011</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="4"/>
-        <v>19232.724566579924</v>
+        <f t="shared" si="2"/>
+        <v>33275</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="1"/>
-        <v>105925.34922016349</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>108876</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="3"/>
+        <v>60500</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="4"/>
+        <v>252501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>32150.418534400003</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>137903.5112064</v>
       </c>
       <c r="D14" s="2">
@@ -48326,7 +48874,7 @@
         <v>497427.06723839999</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>22001</v>
       </c>
       <c r="F14" s="2">
@@ -48334,24 +48882,32 @@
         <v>132012</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="4"/>
-        <v>21641.649234067241</v>
+        <f t="shared" si="2"/>
+        <v>43200</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="1"/>
-        <v>127566.99845423074</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>152076</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="3"/>
+        <v>72000</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="4"/>
+        <v>324501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>39580.502241280003</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>177484.01344767999</v>
       </c>
       <c r="D15" s="2">
@@ -48359,7 +48915,7 @@
         <v>674911.08068608004</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>24001</v>
       </c>
       <c r="F15" s="2">
@@ -48367,24 +48923,32 @@
         <v>156013</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="4"/>
-        <v>24242.562496194205</v>
+        <f t="shared" si="2"/>
+        <v>54925</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
-        <v>151809.56095042493</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>207001</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="3"/>
+        <v>84500</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="4"/>
+        <v>409001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>48496.602689536005</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>225980.61613721598</v>
       </c>
       <c r="D16" s="2">
@@ -48392,7 +48956,7 @@
         <v>900891.69682329602</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>26001</v>
       </c>
       <c r="F16" s="2">
@@ -48400,24 +48964,32 @@
         <v>182014</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="4"/>
-        <v>27056.511103231107</v>
+        <f t="shared" si="2"/>
+        <v>68600</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="1"/>
-        <v>178866.07205365604</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>275601</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="3"/>
+        <v>98000</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="4"/>
+        <v>507001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>59195.923227443207</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>285176.53936465917</v>
       </c>
       <c r="D17" s="2">
@@ -48425,7 +48997,7 @@
         <v>1186068.2361879551</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>28001</v>
       </c>
       <c r="F17" s="2">
@@ -48433,24 +49005,32 @@
         <v>210015</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="4"/>
-        <v>30105.033910343955</v>
+        <f t="shared" si="2"/>
+        <v>84375</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="1"/>
-        <v>208971.10596399999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>359976</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="3"/>
+        <v>112500</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="4"/>
+        <v>619501</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>72035.107872931854</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>357211.64723759104</v>
       </c>
       <c r="D18" s="2">
@@ -48458,7 +49038,7 @@
         <v>1543279.8834255461</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>30001</v>
       </c>
       <c r="F18" s="2">
@@ -48466,24 +49046,32 @@
         <v>240016</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="4"/>
-        <v>33410.136924135702</v>
+        <f t="shared" si="2"/>
+        <v>102400</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="1"/>
-        <v>242381.24288813569</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>462376</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="3"/>
+        <v>128000</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="4"/>
+        <v>747501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>87442.129447518222</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>444653.77668510925</v>
       </c>
       <c r="D19" s="2">
@@ -48491,7 +49079,7 @@
         <v>1987933.6601106552</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>32001</v>
       </c>
       <c r="F19" s="2">
@@ -48499,24 +49087,32 @@
         <v>272017</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="4"/>
-        <v>36994.271219276969</v>
+        <f t="shared" si="2"/>
+        <v>122825</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="1"/>
-        <v>279375.51410741266</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>585201</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="3"/>
+        <v>144500</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="4"/>
+        <v>892001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>105930.55533702187</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>550584.33202213107</v>
       </c>
       <c r="D20" s="2">
@@ -48524,7 +49120,7 @@
         <v>2538517.9921327862</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>34001</v>
       </c>
       <c r="F20" s="2">
@@ -48532,24 +49128,32 @@
         <v>306018</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="4"/>
-        <v>40880.313233446432</v>
+        <f t="shared" si="2"/>
+        <v>145800</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="1"/>
-        <v>320255.8273408591</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>731001</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="3"/>
+        <v>162000</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="4"/>
+        <v>1054001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>128116.66640442624</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>678700.99842655729</v>
       </c>
       <c r="D21" s="2">
@@ -48557,7 +49161,7 @@
         <v>3217218.9905593432</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>36001</v>
       </c>
       <c r="F21" s="2">
@@ -48565,24 +49169,32 @@
         <v>342019</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="4"/>
-        <v>45091.547057523356</v>
+        <f t="shared" si="2"/>
+        <v>171475</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="1"/>
-        <v>365347.37439838244</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>902476</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="3"/>
+        <v>180500</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="4"/>
+        <v>1234501</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>154739.99968531149</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>833440.99811186874</v>
       </c>
       <c r="D22" s="2">
@@ -48590,7 +49202,7 @@
         <v>4050659.988671212</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>38001</v>
       </c>
       <c r="F22" s="2">
@@ -48598,24 +49210,32 @@
         <v>380020</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="4"/>
-        <v>49651.648417852644</v>
+        <f t="shared" si="2"/>
+        <v>200000</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="1"/>
-        <v>414999.02281623508</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1102476</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="3"/>
+        <v>200000</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="4"/>
+        <v>1434501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>186687.99962237378</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1020128.9977342426</v>
       </c>
       <c r="D23" s="2">
@@ -48623,7 +49243,7 @@
         <v>5070788.9864054546</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>40001</v>
       </c>
       <c r="F23" s="2">
@@ -48631,24 +49251,32 @@
         <v>420021</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="4"/>
-        <v>54584.670107231352</v>
+        <f t="shared" si="2"/>
+        <v>231525</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="1"/>
-        <v>469583.69292346644</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1334001</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="3"/>
+        <v>220500</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="4"/>
+        <v>1655001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>225025.59954684853</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1245154.5972810911</v>
       </c>
       <c r="D24" s="2">
@@ -48656,7 +49284,7 @@
         <v>6315943.5836865455</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>42001</v>
       </c>
       <c r="F24" s="2">
@@ -48664,24 +49292,32 @@
         <v>462022</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="4"/>
-        <v>59915.02866684222</v>
+        <f t="shared" si="2"/>
+        <v>266200</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="1"/>
-        <v>529498.72159030871</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1600201</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="3"/>
+        <v>242000</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="4"/>
+        <v>1897001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>271030.71945621824</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1516185.3167373093</v>
       </c>
       <c r="D25" s="2">
@@ -48689,7 +49325,7 @@
         <v>7832128.9004238546</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>44001</v>
       </c>
       <c r="F25" s="2">
@@ -48697,24 +49333,32 @@
         <v>506023</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="4"/>
-        <v>65667.492156608074</v>
+        <f t="shared" si="2"/>
+        <v>304175</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="1"/>
-        <v>595166.21374691674</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1904376</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="3"/>
+        <v>264500</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="4"/>
+        <v>2161501</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>326236.86334746191</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1842422.1800847712</v>
       </c>
       <c r="D26" s="2">
@@ -48722,7 +49366,7 @@
         <v>9674551.0805086251</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>46001</v>
       </c>
       <c r="F26" s="2">
@@ -48730,24 +49374,32 @@
         <v>552024</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="4"/>
-        <v>71867.168879069475</v>
+        <f t="shared" si="2"/>
+        <v>345600</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="1"/>
-        <v>667033.38262598624</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2249976</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="3"/>
+        <v>288000</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="4"/>
+        <v>2449501</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>392484.2360169543</v>
       </c>
       <c r="C27" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2234906.4161017258</v>
       </c>
       <c r="D27" s="2">
@@ -48755,7 +49407,7 @@
         <v>11909457.496610351</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>48001</v>
       </c>
       <c r="F27" s="2">
@@ -48763,24 +49415,32 @@
         <v>600025</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="4"/>
-        <v>78539.496943808801</v>
+        <f t="shared" si="2"/>
+        <v>390625</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="1"/>
-        <v>745572.87956979498</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2640601</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="3"/>
+        <v>312500</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="4"/>
+        <v>2762001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>471981.08322034514</v>
       </c>
       <c r="C28" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2706887.4993220707</v>
       </c>
       <c r="D28" s="2">
@@ -48788,7 +49448,7 @@
         <v>14616344.995932423</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>50001</v>
       </c>
       <c r="F28" s="2">
@@ -48796,24 +49456,32 @@
         <v>650026</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" si="4"/>
-        <v>85710.234577028983</v>
+        <f t="shared" si="2"/>
+        <v>439400</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="1"/>
-        <v>831283.11414682399</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3080001</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="3"/>
+        <v>338000</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="4"/>
+        <v>3100001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>567377.29986441415</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3274264.7991864849</v>
       </c>
       <c r="D29" s="2">
@@ -48821,7 +49489,7 @@
         <v>17890609.795118906</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>52001</v>
       </c>
       <c r="F29" s="2">
@@ -48829,24 +49497,32 @@
         <v>702027</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" si="4"/>
-        <v>93405.451095137178</v>
+        <f t="shared" si="2"/>
+        <v>492075</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" si="1"/>
-        <v>924688.56524196116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3572076</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="3"/>
+        <v>364500</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="4"/>
+        <v>3464501</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>681852.75983729702</v>
       </c>
       <c r="C30" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3956117.5590237817</v>
       </c>
       <c r="D30" s="2">
@@ -48854,7 +49530,7 @@
         <v>21846727.354142688</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>54001</v>
       </c>
       <c r="F30" s="2">
@@ -48862,24 +49538,32 @@
         <v>756028</v>
       </c>
       <c r="G30" s="2">
-        <f t="shared" si="4"/>
-        <v>101651.51847283544</v>
+        <f t="shared" si="2"/>
+        <v>548800</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="1"/>
-        <v>1026340.0837147966</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4120876</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="3"/>
+        <v>392000</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="4"/>
+        <v>3856501</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>819223.31180475641</v>
       </c>
       <c r="C31" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4775340.8708285382</v>
       </c>
       <c r="D31" s="2">
@@ -48887,7 +49571,7 @@
         <v>26622068.224971227</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>56001</v>
       </c>
       <c r="F31" s="2">
@@ -48895,24 +49579,32 @@
         <v>812029</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="4"/>
-        <v>110475.10344581748</v>
+        <f t="shared" si="2"/>
+        <v>609725</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="1"/>
-        <v>1136815.1871606139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4730601</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="3"/>
+        <v>420500</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="4"/>
+        <v>4277001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>984067.97416570771</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5759408.844994246</v>
       </c>
       <c r="D32" s="2">
@@ -48920,7 +49612,7 @@
         <v>32381477.069965474</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>58001</v>
       </c>
       <c r="F32" s="2">
@@ -48928,24 +49620,32 @@
         <v>870030</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="4"/>
-        <v>119903.16009614893</v>
+        <f t="shared" si="2"/>
+        <v>675000</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" si="1"/>
-        <v>1256718.3472567629</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5405601</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="3"/>
+        <v>450000</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="4"/>
+        <v>4727001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1181881.5689988493</v>
       </c>
       <c r="C33" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6941290.413993095</v>
       </c>
       <c r="D33" s="2">
@@ -48953,7 +49653,7 @@
         <v>39322767.483958572</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>60001</v>
       </c>
       <c r="F33" s="2">
@@ -48961,24 +49661,32 @@
         <v>930031</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="4"/>
-        <v>129962.92287508317</v>
+        <f t="shared" si="2"/>
+        <v>744775</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" si="1"/>
-        <v>1386681.270131846</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6150376</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="3"/>
+        <v>480500</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="4"/>
+        <v>5207501</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1419257.8827986191</v>
       </c>
       <c r="C34" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8360548.2967917137</v>
       </c>
       <c r="D34" s="2">
@@ -48986,7 +49694,7 @@
         <v>47683315.78075029</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>62001</v>
       </c>
       <c r="F34" s="2">
@@ -48994,24 +49702,32 @@
         <v>992032</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="4"/>
-        <v>140681.90002368303</v>
+        <f t="shared" si="2"/>
+        <v>819200</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" si="1"/>
-        <v>1527363.1701555289</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6969576</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="3"/>
+        <v>512000</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="4"/>
+        <v>5719501</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1704109.4593583429</v>
       </c>
       <c r="C35" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>10064657.756150056</v>
       </c>
       <c r="D35" s="2">
@@ -49019,7 +49735,7 @@
         <v>57747973.536900342</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>64001</v>
       </c>
       <c r="F35" s="2">
@@ -49027,24 +49743,32 @@
         <v>1056033</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" si="4"/>
-        <v>152087.86735638179</v>
+        <f t="shared" si="2"/>
+        <v>898425</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" si="1"/>
-        <v>1679451.0375119108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7868001</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="3"/>
+        <v>544500</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="4"/>
+        <v>6264001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2045931.3512300116</v>
       </c>
       <c r="C36" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>12110589.107380068</v>
       </c>
       <c r="D36" s="2">
@@ -49052,7 +49776,7 @@
         <v>69858562.644280404</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>66001</v>
       </c>
       <c r="F36" s="2">
@@ -49060,24 +49784,32 @@
         <v>1122034</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="4"/>
-        <v>164208.86237667289</v>
+        <f t="shared" si="2"/>
+        <v>982600</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" si="1"/>
-        <v>1843659.8998885837</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8850601</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="3"/>
+        <v>578000</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="4"/>
+        <v>6842001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2456117.6214760137</v>
       </c>
       <c r="C37" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>14566706.728856081</v>
       </c>
       <c r="D37" s="2">
@@ -49085,7 +49817,7 @@
         <v>84425269.373136491</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>68001</v>
       </c>
       <c r="F37" s="2">
@@ -49093,24 +49825,32 @@
         <v>1190035</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" si="4"/>
-        <v>177073.17869759607</v>
+        <f t="shared" si="2"/>
+        <v>1071875</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" si="1"/>
-        <v>2020733.0785861798</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9922476</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="3"/>
+        <v>612500</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="4"/>
+        <v>7454501</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2948341.1457712166</v>
       </c>
       <c r="C38" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>17515047.8746273</v>
       </c>
       <c r="D38" s="2">
@@ -49118,7 +49858,7 @@
         <v>101940317.24776378</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>70001</v>
       </c>
       <c r="F38" s="2">
@@ -49126,24 +49866,32 @@
         <v>1260036</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="4"/>
-        <v>190709.36074268064</v>
+        <f t="shared" si="2"/>
+        <v>1166400</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" si="1"/>
-        <v>2211442.4393288605</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>11088876</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="3"/>
+        <v>648000</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="4"/>
+        <v>8102501</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3539009.3749254597</v>
       </c>
       <c r="C39" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>21054057.24955276</v>
       </c>
       <c r="D39" s="2">
@@ -49151,7 +49899,7 @@
         <v>122994374.49731654</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>72001</v>
       </c>
       <c r="F39" s="2">
@@ -49159,24 +49907,32 @@
         <v>1332037</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" si="4"/>
-        <v>205146.19870558815</v>
+        <f t="shared" si="2"/>
+        <v>1266325</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="1"/>
-        <v>2416588.6380344485</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12355201</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="3"/>
+        <v>684500</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="4"/>
+        <v>8787001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4247811.2499105521</v>
       </c>
       <c r="C40" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>25301868.499463312</v>
       </c>
       <c r="D40" s="2">
@@ -49184,7 +49940,7 @@
         <v>148296242.99677986</v>
       </c>
       <c r="E40" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>74001</v>
       </c>
       <c r="F40" s="2">
@@ -49192,24 +49948,32 @@
         <v>1406038</v>
       </c>
       <c r="G40" s="2">
-        <f t="shared" si="4"/>
-        <v>220412.7237489532</v>
+        <f t="shared" si="2"/>
+        <v>1371800</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" si="1"/>
-        <v>2637001.3617834016</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>13727001</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="3"/>
+        <v>722000</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="4"/>
+        <v>9509001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5098373.4998926623</v>
       </c>
       <c r="C41" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>30400241.999355976</v>
       </c>
       <c r="D41" s="2">
@@ -49217,7 +49981,7 @@
         <v>178696484.99613583</v>
       </c>
       <c r="E41" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>76001</v>
       </c>
       <c r="F41" s="2">
@@ -49225,24 +49989,32 @@
         <v>1482039</v>
       </c>
       <c r="G41" s="2">
-        <f t="shared" si="4"/>
-        <v>236538.20342487987</v>
+        <f t="shared" si="2"/>
+        <v>1482975</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" si="1"/>
-        <v>2873539.5652082814</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15209976</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="3"/>
+        <v>760500</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="4"/>
+        <v>10269501</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6119048.1998711945</v>
       </c>
       <c r="C42" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>36519290.199227169</v>
       </c>
       <c r="D42" s="2">
@@ -49250,7 +50022,7 @@
         <v>215215775.19536299</v>
       </c>
       <c r="E42" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>78001</v>
       </c>
       <c r="F42" s="2">
@@ -49258,24 +50030,32 @@
         <v>1560040</v>
       </c>
       <c r="G42" s="2">
-        <f t="shared" si="4"/>
-        <v>253552.13730126186</v>
+        <f t="shared" si="2"/>
+        <v>1600000</v>
       </c>
       <c r="H42" s="2">
         <f t="shared" si="1"/>
-        <v>3127091.7025095434</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16809976</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="3"/>
+        <v>800000</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="4"/>
+        <v>11069501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7343857.8398454338</v>
       </c>
       <c r="C43" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>43863148.039072603</v>
       </c>
       <c r="D43" s="2">
@@ -49283,7 +50063,7 @@
         <v>259078923.23443559</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>80001</v>
       </c>
       <c r="F43" s="2">
@@ -49291,24 +50071,32 @@
         <v>1640041</v>
       </c>
       <c r="G43" s="2">
-        <f t="shared" si="4"/>
-        <v>271484.25277961418</v>
+        <f t="shared" si="2"/>
+        <v>1723025</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" si="1"/>
-        <v>3398575.9552891576</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18533001</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="3"/>
+        <v>840500</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="4"/>
+        <v>11910001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8813629.4078145213</v>
       </c>
       <c r="C44" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>52676777.446887121</v>
       </c>
       <c r="D44" s="2">
@@ -49316,7 +50104,7 @@
         <v>311755700.68132269</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>82001</v>
       </c>
       <c r="F44" s="2">
@@ -49324,24 +50112,32 @@
         <v>1722042</v>
       </c>
       <c r="G44" s="2">
-        <f t="shared" si="4"/>
-        <v>290364.50109142601</v>
+        <f t="shared" si="2"/>
+        <v>1852200</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" si="1"/>
-        <v>3688940.4563805833</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20385201</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="3"/>
+        <v>882000</v>
+      </c>
+      <c r="J44" s="2">
+        <f t="shared" si="4"/>
+        <v>12792001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10577355.289377425</v>
       </c>
       <c r="C45" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>63254132.736264542</v>
       </c>
       <c r="D45" s="2">
@@ -49349,7 +50145,7 @@
         <v>375009833.41758722</v>
       </c>
       <c r="E45" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>84001</v>
       </c>
       <c r="F45" s="2">
@@ -49357,24 +50153,32 @@
         <v>1806043</v>
       </c>
       <c r="G45" s="2">
-        <f t="shared" si="4"/>
-        <v>310223.05346122826</v>
+        <f t="shared" si="2"/>
+        <v>1987675</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" si="1"/>
-        <v>3999163.5098418118</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22372876</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="3"/>
+        <v>924500</v>
+      </c>
+      <c r="J45" s="2">
+        <f t="shared" si="4"/>
+        <v>13716501</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>12693826.347252909</v>
       </c>
       <c r="C46" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>75947959.083517447</v>
       </c>
       <c r="D46" s="2">
@@ -49382,7 +50186,7 @@
         <v>450957792.50110465</v>
       </c>
       <c r="E46" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>86001</v>
       </c>
       <c r="F46" s="2">
@@ -49390,24 +50194,32 @@
         <v>1892044</v>
       </c>
       <c r="G46" s="2">
-        <f t="shared" si="4"/>
-        <v>331090.29742560833</v>
+        <f t="shared" si="2"/>
+        <v>2129600</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" si="1"/>
-        <v>4330253.80726742</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24502476</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="3"/>
+        <v>968000</v>
+      </c>
+      <c r="J46" s="2">
+        <f t="shared" si="4"/>
+        <v>14684501</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>15233591.616703492</v>
       </c>
       <c r="C47" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>91181550.700220942</v>
       </c>
       <c r="D47" s="2">
@@ -49415,7 +50227,7 @@
         <v>542139343.20132565</v>
       </c>
       <c r="E47" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>88001</v>
       </c>
       <c r="F47" s="2">
@@ -49423,24 +50235,32 @@
         <v>1980045</v>
       </c>
       <c r="G47" s="2">
-        <f t="shared" si="4"/>
-        <v>352996.83329834224</v>
+        <f t="shared" si="2"/>
+        <v>2278125</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" si="1"/>
-        <v>4683250.6405657623</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26780601</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="3"/>
+        <v>1012500</v>
+      </c>
+      <c r="J47" s="2">
+        <f t="shared" si="4"/>
+        <v>15697001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18281309.940044191</v>
       </c>
       <c r="C48" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>109462860.64026514</v>
       </c>
       <c r="D48" s="2">
@@ -49448,7 +50268,7 @@
         <v>651602203.84159076</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>90001</v>
       </c>
       <c r="F48" s="2">
@@ -49456,24 +50276,32 @@
         <v>2070046</v>
       </c>
       <c r="G48" s="2">
-        <f t="shared" si="4"/>
-        <v>375973.47077263665</v>
+        <f t="shared" si="2"/>
+        <v>2433400</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" si="1"/>
-        <v>5059224.1113383994</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29214001</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="3"/>
+        <v>1058000</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" si="4"/>
+        <v>16755001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>21938571.928053029</v>
       </c>
       <c r="C49" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>131401432.56831816</v>
       </c>
       <c r="D49" s="2">
@@ -49481,7 +50309,7 @@
         <v>783003636.40990889</v>
       </c>
       <c r="E49" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>92001</v>
       </c>
       <c r="F49" s="2">
@@ -49489,24 +50317,32 @@
         <v>2162047</v>
       </c>
       <c r="G49" s="2">
-        <f t="shared" si="4"/>
-        <v>400051.22565222369</v>
+        <f t="shared" si="2"/>
+        <v>2595575</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" si="1"/>
-        <v>5459275.3369906228</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31809576</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="3"/>
+        <v>1104500</v>
+      </c>
+      <c r="J49" s="2">
+        <f t="shared" si="4"/>
+        <v>17859501</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>26327286.313663635</v>
       </c>
       <c r="C50" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>157728718.88198179</v>
       </c>
       <c r="D50" s="2">
@@ -49514,7 +50350,7 @@
         <v>940732355.29189062</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>94001</v>
       </c>
       <c r="F50" s="2">
@@ -49522,24 +50358,32 @@
         <v>2256048</v>
       </c>
       <c r="G50" s="2">
-        <f t="shared" si="4"/>
-        <v>425261.31670371996</v>
+        <f t="shared" si="2"/>
+        <v>2764800</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" si="1"/>
-        <v>5884536.6536943428</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>34574376</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="3"/>
+        <v>1152000</v>
+      </c>
+      <c r="J50" s="2">
+        <f t="shared" si="4"/>
+        <v>19011501</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>31593743.576396361</v>
       </c>
       <c r="C51" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>189322462.45837814</v>
       </c>
       <c r="D51" s="2">
@@ -49547,7 +50391,7 @@
         <v>1130054817.7502687</v>
       </c>
       <c r="E51" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>96001</v>
       </c>
       <c r="F51" s="2">
@@ -49555,24 +50399,32 @@
         <v>2352049</v>
       </c>
       <c r="G51" s="2">
-        <f t="shared" si="4"/>
-        <v>451635.16262324178</v>
+        <f t="shared" si="2"/>
+        <v>2941225</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" si="1"/>
-        <v>6336171.8163175844</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37515601</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="3"/>
+        <v>1200500</v>
+      </c>
+      <c r="J51" s="2">
+        <f t="shared" si="4"/>
+        <v>20212001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>37913492.291675635</v>
       </c>
       <c r="C52" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>227235954.75005376</v>
       </c>
       <c r="D52" s="2">
@@ -49580,7 +50432,7 @@
         <v>1357290772.5003223</v>
       </c>
       <c r="E52" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>98001</v>
       </c>
       <c r="F52" s="2">
@@ -49588,24 +50440,32 @@
         <v>2450050</v>
       </c>
       <c r="G52" s="2">
-        <f t="shared" si="4"/>
-        <v>479204.37911084824</v>
+        <f t="shared" si="2"/>
+        <v>3125000</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" si="1"/>
-        <v>6815376.1954284329</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>40640601</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="3"/>
+        <v>1250000</v>
+      </c>
+      <c r="J52" s="2">
+        <f t="shared" si="4"/>
+        <v>21462001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>45497190.750010759</v>
       </c>
       <c r="C53" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>272733145.50006449</v>
       </c>
       <c r="D53" s="2">
@@ -49613,7 +50473,7 @@
         <v>1630023918.0003867</v>
       </c>
       <c r="E53" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>100001</v>
       </c>
       <c r="F53" s="2">
@@ -49621,24 +50481,32 @@
         <v>2550051</v>
       </c>
       <c r="G53" s="2">
-        <f t="shared" si="4"/>
-        <v>508000.77604682645</v>
+        <f t="shared" si="2"/>
+        <v>3316275</v>
       </c>
       <c r="H53" s="2">
         <f t="shared" si="1"/>
-        <v>7323376.9714752594</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43956876</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="3"/>
+        <v>1300500</v>
+      </c>
+      <c r="J53" s="2">
+        <f t="shared" si="4"/>
+        <v>22762501</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>54597628.90001291</v>
       </c>
       <c r="C54" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>327330774.4000774</v>
       </c>
       <c r="D54" s="2">
@@ -49646,7 +50514,7 @@
         <v>1957354692.4004641</v>
       </c>
       <c r="E54" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>102001</v>
       </c>
       <c r="F54" s="2">
@@ -49654,24 +50522,32 @@
         <v>2652052</v>
       </c>
       <c r="G54" s="2">
-        <f t="shared" si="4"/>
-        <v>538056.35476431798</v>
+        <f t="shared" si="2"/>
+        <v>3515200</v>
       </c>
       <c r="H54" s="2">
         <f t="shared" si="1"/>
-        <v>7861433.3262395775</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>47472076</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="3"/>
+        <v>1352000</v>
+      </c>
+      <c r="J54" s="2">
+        <f t="shared" si="4"/>
+        <v>24114501</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>65518154.680015489</v>
       </c>
       <c r="C55" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>392848929.08009291</v>
       </c>
       <c r="D55" s="2">
@@ -49679,7 +50555,7 @@
         <v>2350203621.480557</v>
       </c>
       <c r="E55" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>104001</v>
       </c>
       <c r="F55" s="2">
@@ -49687,24 +50563,32 @@
         <v>2756053</v>
       </c>
       <c r="G55" s="2">
-        <f t="shared" si="4"/>
-        <v>569403.30541315547</v>
+        <f t="shared" si="2"/>
+        <v>3721925</v>
       </c>
       <c r="H55" s="2">
         <f t="shared" si="1"/>
-        <v>8430836.6316527333</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>51194001</v>
+      </c>
+      <c r="I55" s="2">
+        <f t="shared" si="3"/>
+        <v>1404500</v>
+      </c>
+      <c r="J55" s="2">
+        <f t="shared" si="4"/>
+        <v>25519001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>78622785.616018593</v>
       </c>
       <c r="C56" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>471471714.6961115</v>
       </c>
       <c r="D56" s="2">
@@ -49712,7 +50596,7 @@
         <v>2821675336.1766686</v>
       </c>
       <c r="E56" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>106001</v>
       </c>
       <c r="F56" s="2">
@@ -49720,24 +50604,32 @@
         <v>2862054</v>
       </c>
       <c r="G56" s="2">
-        <f t="shared" si="4"/>
-        <v>602074.00441016629</v>
+        <f t="shared" si="2"/>
+        <v>3936600</v>
       </c>
       <c r="H56" s="2">
         <f t="shared" si="1"/>
-        <v>9032910.6360628996</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>55130601</v>
+      </c>
+      <c r="I56" s="2">
+        <f t="shared" si="3"/>
+        <v>1458000</v>
+      </c>
+      <c r="J56" s="2">
+        <f t="shared" si="4"/>
+        <v>26977001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>94348342.739222318</v>
       </c>
       <c r="C57" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>565820057.43533385</v>
       </c>
       <c r="D57" s="2">
@@ -49745,7 +50637,7 @@
         <v>3387495393.6120024</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>108001</v>
       </c>
       <c r="F57" s="2">
@@ -49753,24 +50645,32 @@
         <v>2970055</v>
       </c>
       <c r="G57" s="2">
-        <f t="shared" si="4"/>
-        <v>636101.01197151467</v>
+        <f t="shared" si="2"/>
+        <v>4159375</v>
       </c>
       <c r="H57" s="2">
         <f t="shared" si="1"/>
-        <v>9669011.6480344143</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59289976</v>
+      </c>
+      <c r="I57" s="2">
+        <f t="shared" si="3"/>
+        <v>1512500</v>
+      </c>
+      <c r="J57" s="2">
+        <f t="shared" si="4"/>
+        <v>28489501</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>113219011.28706679</v>
       </c>
       <c r="C58" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>679039068.72240067</v>
       </c>
       <c r="D58" s="2">
@@ -49778,7 +50678,7 @@
         <v>4066534462.334403</v>
       </c>
       <c r="E58" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>110001</v>
       </c>
       <c r="F58" s="2">
@@ -49786,24 +50686,32 @@
         <v>3080056</v>
       </c>
       <c r="G58" s="2">
-        <f t="shared" si="4"/>
-        <v>671517.06972298003</v>
+        <f t="shared" si="2"/>
+        <v>4390400</v>
       </c>
       <c r="H58" s="2">
         <f t="shared" si="1"/>
-        <v>10340528.717757395</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63680376</v>
+      </c>
+      <c r="I58" s="2">
+        <f t="shared" si="3"/>
+        <v>1568000</v>
+      </c>
+      <c r="J58" s="2">
+        <f t="shared" si="4"/>
+        <v>30057501</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>135863813.54448014</v>
       </c>
       <c r="C59" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>814902882.26688075</v>
       </c>
       <c r="D59" s="2">
@@ -49811,7 +50719,7 @@
         <v>4881437344.601284</v>
       </c>
       <c r="E59" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>112001</v>
       </c>
       <c r="F59" s="2">
@@ -49819,24 +50727,32 @@
         <v>3192057</v>
       </c>
       <c r="G59" s="2">
-        <f t="shared" si="4"/>
-        <v>708355.0983843162</v>
+        <f t="shared" si="2"/>
+        <v>4629825</v>
       </c>
       <c r="H59" s="2">
         <f t="shared" si="1"/>
-        <v>11048883.816141712</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68310201</v>
+      </c>
+      <c r="I59" s="2">
+        <f t="shared" si="3"/>
+        <v>1624500</v>
+      </c>
+      <c r="J59" s="2">
+        <f t="shared" si="4"/>
+        <v>31682001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>163037576.25337619</v>
       </c>
       <c r="C60" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>977940458.520257</v>
       </c>
       <c r="D60" s="2">
@@ -49844,7 +50760,7 @@
         <v>5859377803.121541</v>
       </c>
       <c r="E60" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>114001</v>
       </c>
       <c r="F60" s="2">
@@ -49852,24 +50768,32 @@
         <v>3306058</v>
       </c>
       <c r="G60" s="2">
-        <f t="shared" si="4"/>
-        <v>746648.19552412792</v>
+        <f t="shared" si="2"/>
+        <v>4877800</v>
       </c>
       <c r="H60" s="2">
         <f t="shared" si="1"/>
-        <v>11795532.01166584</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73188001</v>
+      </c>
+      <c r="I60" s="2">
+        <f t="shared" si="3"/>
+        <v>1682000</v>
+      </c>
+      <c r="J60" s="2">
+        <f t="shared" si="4"/>
+        <v>33364001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>195646091.50405142</v>
       </c>
       <c r="C61" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1173586550.0243084</v>
       </c>
       <c r="D61" s="2">
@@ -49877,7 +50801,7 @@
         <v>7032964353.1458492</v>
       </c>
       <c r="E61" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>116001</v>
       </c>
       <c r="F61" s="2">
@@ -49885,24 +50809,32 @@
         <v>3422059</v>
       </c>
       <c r="G61" s="2">
-        <f t="shared" si="4"/>
-        <v>786429.63338189654</v>
+        <f t="shared" si="2"/>
+        <v>5134475</v>
       </c>
       <c r="H61" s="2">
         <f t="shared" si="1"/>
-        <v>12581961.645047735</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78322476</v>
+      </c>
+      <c r="I61" s="2">
+        <f t="shared" si="3"/>
+        <v>1740500</v>
+      </c>
+      <c r="J61" s="2">
+        <f t="shared" si="4"/>
+        <v>35104501</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>234776309.80486169</v>
       </c>
       <c r="C62" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1408362859.8291702</v>
       </c>
       <c r="D62" s="2">
@@ -49910,7 +50842,7 @@
         <v>8441327212.9750195</v>
       </c>
       <c r="E62" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>118001</v>
       </c>
       <c r="F62" s="2">
@@ -49918,24 +50850,32 @@
         <v>3540060</v>
       </c>
       <c r="G62" s="2">
-        <f t="shared" si="4"/>
-        <v>827732.85675402719</v>
+        <f t="shared" si="2"/>
+        <v>5400000</v>
       </c>
       <c r="H62" s="2">
         <f t="shared" si="1"/>
-        <v>13409694.501801763</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>83722476</v>
+      </c>
+      <c r="I62" s="2">
+        <f t="shared" si="3"/>
+        <v>1800000</v>
+      </c>
+      <c r="J62" s="2">
+        <f t="shared" si="4"/>
+        <v>36904501</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>281732571.76583403</v>
       </c>
       <c r="C63" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1690095431.5950043</v>
       </c>
       <c r="D63" s="2">
@@ -49943,7 +50883,7 @@
         <v>10131422644.570024</v>
       </c>
       <c r="E63" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>120001</v>
       </c>
       <c r="F63" s="2">
@@ -49951,24 +50891,32 @@
         <v>3660061</v>
       </c>
       <c r="G63" s="2">
-        <f t="shared" si="4"/>
-        <v>870591.48094099003</v>
+        <f t="shared" si="2"/>
+        <v>5674525</v>
       </c>
       <c r="H63" s="2">
         <f t="shared" si="1"/>
-        <v>14280285.982742753</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>89397001</v>
+      </c>
+      <c r="I63" s="2">
+        <f t="shared" si="3"/>
+        <v>1860500</v>
+      </c>
+      <c r="J63" s="2">
+        <f t="shared" si="4"/>
+        <v>38765001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>338080086.11900085</v>
       </c>
       <c r="C64" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2028175517.7140052</v>
       </c>
       <c r="D64" s="2">
@@ -49976,7 +50924,7 @@
         <v>12159598162.284029</v>
       </c>
       <c r="E64" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>122001</v>
       </c>
       <c r="F64" s="2">
@@ -49984,29 +50932,44 @@
         <v>3782062</v>
       </c>
       <c r="G64" s="2">
-        <f t="shared" si="4"/>
-        <v>915039.28975276963</v>
+        <f>$G$66*A64^$G$67</f>
+        <v>5958200</v>
       </c>
       <c r="H64" s="2">
         <f t="shared" si="1"/>
-        <v>15195325.272495523</v>
-      </c>
-    </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+        <v>95355201</v>
+      </c>
+      <c r="I64" s="2">
+        <f>$I$66*A64^$I$67</f>
+        <v>1922000</v>
+      </c>
+      <c r="J64" s="2">
+        <f t="shared" si="4"/>
+        <v>40687001</v>
+      </c>
+    </row>
+    <row r="66" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G66" s="2">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I66" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="67" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G67" s="8">
-        <v>3.3</v>
+        <v>3</v>
+      </c>
+      <c r="I67" s="8">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -50017,8 +50980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A64194-8C09-4F9D-A9F0-F80B6ABDA2F2}">
   <dimension ref="B2:J342"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50119,8 +51082,11 @@
         <v>10</v>
       </c>
       <c r="I8">
-        <f>($C$3-0.5)</f>
+        <f>($C$3-0.5)*J8</f>
         <v>4.5</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -58497,7 +59463,7 @@
         <v>0</v>
       </c>
       <c r="I332" s="10">
-        <f t="shared" ref="I332:I395" si="27">IF(B332&gt;=$J$9,0,J332)</f>
+        <f t="shared" ref="I332:I342" si="27">IF(B332&gt;=$J$9,0,J332)</f>
         <v>0</v>
       </c>
       <c r="J332" s="11">

</xml_diff>